<commit_message>
hopefully right calculation for faktor real world env
</commit_message>
<xml_diff>
--- a/BerechnungenDatenExperiment.xlsx
+++ b/BerechnungenDatenExperiment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Entfernung vom Schanir</t>
   </si>
@@ -93,25 +93,55 @@
     <t xml:space="preserve">Hebt ab</t>
   </si>
   <si>
-    <t xml:space="preserve">Auftrieb in N</t>
+    <t>Auftrieb</t>
   </si>
   <si>
-    <t xml:space="preserve">Gewicht eines Drohnenarms in kg</t>
+    <t>N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gewicht eines Drohnenarms</t>
+  </si>
+  <si>
+    <t>kg</t>
   </si>
   <si>
     <t xml:space="preserve">Beschleunigung bei maximalem Auftrieb</t>
   </si>
   <si>
-    <t xml:space="preserve">maximaler output des controllers</t>
+    <t>m/s²</t>
   </si>
   <si>
-    <t xml:space="preserve">Faktor für Simulation</t>
+    <t xml:space="preserve">output range des controllers</t>
   </si>
   <si>
-    <t>m/s³</t>
+    <t>output</t>
   </si>
   <si>
-    <t>winkel/s³</t>
+    <t xml:space="preserve">Faktor für Simulation in Metern</t>
+  </si>
+  <si>
+    <t>m/(s²*output)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Länge eines Arms</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Umfang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grad pro Meter Drohnenarm</t>
+  </si>
+  <si>
+    <t>°/m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faktor in Winkel</t>
+  </si>
+  <si>
+    <t>winkel/(s²*output)</t>
   </si>
 </sst>
 </file>
@@ -7555,7 +7585,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="100" workbookViewId="0">
       <selection activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -7854,7 +7884,7 @@
         <v>22</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" ref="K16:K21" si="6">-I16*9.81</f>
+        <f t="shared" ref="K16:K20" si="6">-I16*9.81</f>
         <v>240.04643478260846</v>
       </c>
       <c r="L16" s="4">
@@ -8074,7 +8104,7 @@
         <v>-1041.8608695652174</v>
       </c>
       <c r="K21" s="4">
-        <f t="shared" si="6"/>
+        <f>-I21*9.81</f>
         <v>10220.655130434783</v>
       </c>
       <c r="L21" s="4">
@@ -8087,91 +8117,151 @@
     <row r="22">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" ht="14.25"/>
+    <row r="23" ht="14.25">
+      <c r="K23">
+        <f>K21/1000</f>
+        <v>10.220655130434784</v>
+      </c>
+    </row>
     <row r="24">
       <c r="A24" s="1"/>
-      <c r="E24" t="s">
+      <c r="C24" t="s">
         <v>23</v>
       </c>
       <c r="G24">
         <f>G21/1000*9.81</f>
         <v>4.7624137826086956</v>
       </c>
+      <c r="H24" t="s">
+        <v>24</v>
+      </c>
+      <c r="K24">
+        <f>K23/4</f>
+        <v>2.5551637826086959</v>
+      </c>
     </row>
     <row r="25">
-      <c r="B25" t="s">
+      <c r="A25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" t="s">
-        <v>24</v>
+      <c r="C25" t="s">
+        <v>25</v>
       </c>
       <c r="G25">
         <f>0.9/4</f>
         <v>0.22500000000000001</v>
       </c>
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="1"/>
-      <c r="B26" t="s">
+      <c r="A26" t="s">
         <v>11</v>
       </c>
-      <c r="G26" t="s">
-        <v>25</v>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26">
+        <f>G24/G25</f>
+        <v>21.166283478260869</v>
+      </c>
+      <c r="H26" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" ht="14.25">
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
       <c r="G27">
-        <f>G24/G25</f>
-        <v>21.166283478260869</v>
+        <v>1000</v>
+      </c>
+      <c r="H27" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1"/>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28">
+        <f>G26/G27</f>
+        <v>0.021166283478260869</v>
+      </c>
+      <c r="H28" t="s">
+        <v>32</v>
+      </c>
       <c r="I28" s="6"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="D29" t="s">
-        <v>26</v>
+      <c r="C29" t="s">
+        <v>33</v>
       </c>
       <c r="G29">
-        <v>1000</v>
+        <v>0.25</v>
+      </c>
+      <c r="H29" t="s">
+        <v>34</v>
       </c>
       <c r="I29" s="7"/>
     </row>
     <row r="30">
       <c r="A30" s="1"/>
-      <c r="G30" t="s">
-        <v>27</v>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30">
+        <f>2*PI()*G29</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="H30" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="31" ht="14.25">
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
       <c r="G31">
-        <f>G27/G29</f>
-        <v>0.021166283478260869</v>
+        <f>360/G30</f>
+        <v>229.18311805232929</v>
       </c>
       <c r="H31" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1"/>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32">
+        <f>G28*G31</f>
+        <v>4.8509548451273279</v>
+      </c>
+      <c r="H32" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="33" ht="14.25">
-      <c r="G33">
-        <v>0.25</v>
-      </c>
-      <c r="H33" t="s">
-        <v>29</v>
-      </c>
-    </row>
+    <row r="33" ht="14.25"/>
     <row r="34">
       <c r="A34" s="1"/>
     </row>
+    <row r="35" ht="14.25"/>
     <row r="36">
       <c r="A36" s="1"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="I37" s="6"/>
     </row>
     <row r="38">
       <c r="A38" s="1"/>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="G39" s="7"/>
     </row>
     <row r="40">
       <c r="A40" s="1"/>

</xml_diff>